<commit_message>
update claim sub type valueset
</commit_message>
<xml_diff>
--- a/v0.7.1/StructureDefinition-ClaimResponse.xlsx
+++ b/v0.7.1/StructureDefinition-ClaimResponse.xlsx
@@ -536,7 +536,7 @@
     <t>A more granular claim typecode.</t>
   </si>
   <si>
-    <t>https://staging-hcx.swasth.app/hapi-fhir/fhir/ValueSet/hcx-admission-types</t>
+    <t>https://staging-hcx.swasth.app/hapi-fhir/fhir/ValueSet/hcx-claim-sub-types</t>
   </si>
   <si>
     <t>ClaimResponse.use</t>
@@ -2219,7 +2219,7 @@
     <col min="23" max="23" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.9609375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="120.6484375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="71.2578125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="71.1953125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="20.84375" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="18.84765625" customWidth="true" bestFit="true"/>

</xml_diff>